<commit_message>
Ajout modification des notes d'un dossier
</commit_message>
<xml_diff>
--- a/FichesTemps/MaximeAubin4.xlsx
+++ b/FichesTemps/MaximeAubin4.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36D6872-5B07-4851-8F4F-E9C0C868BD87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C92D52B-EB2B-4CD3-93AD-C9E38FAFB7F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="bsnEa0N1OcI6znPoPEcq3AHEi57LtmD/hoPfLk9LAHbO8ZgF/KxDU64xoRN551lSOgXhKiKNTKiOVsg9sOO7CQ==" workbookSaltValue="Arsw55Oy1Kl5wQ7vU+yWcQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="101">
   <si>
     <t>Fiche d'évaluation du travail d'équipe</t>
   </si>
@@ -434,6 +434,21 @@
   </si>
   <si>
     <t>Fix bug de merging</t>
+  </si>
+  <si>
+    <t>16/02/2023</t>
+  </si>
+  <si>
+    <t>Mettre en ordre la liste des requêtes</t>
+  </si>
+  <si>
+    <t>Rencontre client</t>
+  </si>
+  <si>
+    <t>Modification des note d'un dossier</t>
+  </si>
+  <si>
+    <t>Ajout de la documentation des nouvelle méthode de DossierController</t>
   </si>
 </sst>
 </file>
@@ -1833,7 +1848,7 @@
   <dimension ref="A1:F466"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1926,7 +1941,7 @@
       </c>
       <c r="C9" s="47">
         <f>SUM(C11:C466)</f>
-        <v>11</v>
+        <v>16.5</v>
       </c>
       <c r="D9" s="46" t="s">
         <v>64</v>
@@ -2094,28 +2109,52 @@
       <c r="D23" s="52"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="51"/>
+      <c r="A24" s="48" t="s">
+        <v>96</v>
+      </c>
       <c r="B24" s="52"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="52"/>
+      <c r="C24" s="53">
+        <v>0.25</v>
+      </c>
+      <c r="D24" s="52" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="51"/>
+      <c r="A25" s="48" t="s">
+        <v>96</v>
+      </c>
       <c r="B25" s="52"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="52"/>
+      <c r="C25" s="53">
+        <v>0.75</v>
+      </c>
+      <c r="D25" s="52" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="51"/>
+      <c r="A26" s="48" t="s">
+        <v>96</v>
+      </c>
       <c r="B26" s="52"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="52"/>
+      <c r="C26" s="53">
+        <v>4</v>
+      </c>
+      <c r="D26" s="52" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="51"/>
+      <c r="A27" s="48" t="s">
+        <v>96</v>
+      </c>
       <c r="B27" s="52"/>
-      <c r="C27" s="53"/>
-      <c r="D27" s="52"/>
+      <c r="C27" s="53">
+        <v>0.5</v>
+      </c>
+      <c r="D27" s="52" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="51"/>

</xml_diff>

<commit_message>
Documentation et feuille de temps
</commit_message>
<xml_diff>
--- a/FichesTemps/MaximeAubin4.xlsx
+++ b/FichesTemps/MaximeAubin4.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C92D52B-EB2B-4CD3-93AD-C9E38FAFB7F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA30A006-D072-4498-A265-122E56408323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="bsnEa0N1OcI6znPoPEcq3AHEi57LtmD/hoPfLk9LAHbO8ZgF/KxDU64xoRN551lSOgXhKiKNTKiOVsg9sOO7CQ==" workbookSaltValue="Arsw55Oy1Kl5wQ7vU+yWcQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="105">
   <si>
     <t>Fiche d'évaluation du travail d'équipe</t>
   </si>
@@ -382,21 +382,6 @@
     <t>Rencontre d'équipe</t>
   </si>
   <si>
-    <t>Cette fois je suis beaucoup plus fier du résultat que j'ai produit. Je crois cependant que j'ai pris trop de temps a faire certaine tâche</t>
-  </si>
-  <si>
-    <t>La seul raison que j'ai pas mis 5 pour la ligne "a aidé l'équipe à prendre des décision" c'est parce qu'il n'a pas parlé tant que ça quand on parlais de ce a quoi on voulait qu'un module ressemble</t>
-  </si>
-  <si>
-    <t>Jean-philippe a pris un des développement qui me causait des problèmes et s'en est occupé avec brio, cela m'a permit de terminer d'autre tâche a la place de rester bloqué</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Karl a bien travailler cette semaine. Il a régler beaucoup  de problèmes que l'on avait dans l'API </t>
-  </si>
-  <si>
-    <t>Je n'ai aucune reproche a Victor, il a aidé Karl a régler les problèmes d'API, et a bien travaillé sur l'application</t>
-  </si>
-  <si>
     <t>13/02/2023</t>
   </si>
   <si>
@@ -445,10 +430,37 @@
     <t>Rencontre client</t>
   </si>
   <si>
-    <t>Modification des note d'un dossier</t>
-  </si>
-  <si>
     <t>Ajout de la documentation des nouvelle méthode de DossierController</t>
+  </si>
+  <si>
+    <t>19/02/2023</t>
+  </si>
+  <si>
+    <t>Documentation des tâches que les prochains programmeurs auraient a faire</t>
+  </si>
+  <si>
+    <t>Modification des note d'un dossier (coté visuel)</t>
+  </si>
+  <si>
+    <t>Modification des notes d'un dossier (appel à l'API)</t>
+  </si>
+  <si>
+    <t>Toute la documentation que je devais produire à été complété à temps et j'ai même réussit à terminer des finitions dans l'applications dans les temps</t>
+  </si>
+  <si>
+    <t>Il a complété la création de requête, ce qui était le plus gros morceau de l'application. Il a très bien travaillé</t>
+  </si>
+  <si>
+    <t>La visualisation des résultats et ses tests ont été complété avec succès dans les temps. Il a même été retoucher certains de ses anciens développement pour simplifier la vie des utilisateurs</t>
+  </si>
+  <si>
+    <t>Karl a terminé tous les documents de planification nécessaire cette semaine. De plus, il a ajouter des alerte pour empêcher les utilisateur de faire des gafes et il a ajouter la validation des formulaire</t>
+  </si>
+  <si>
+    <t>A complété la création des résultats, ce qui était aussi un gros morceau de l'application. Il a modifié l'application pour que tout soit uniforme (coté visuel et code)</t>
+  </si>
+  <si>
+    <t>Feuille de temps</t>
   </si>
 </sst>
 </file>
@@ -1847,8 +1859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B1E992-A4D6-4269-AA92-453ABD10AC9B}">
   <dimension ref="A1:F466"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1925,8 +1937,8 @@
       <c r="C8" s="56"/>
       <c r="D8" s="38" t="str">
         <f>_xlfn.CONCAT("Évaluateur = ",Évaluateur!F14," ",Évaluateur!D30,CHAR(10),'Coéquipier 1'!D9:I9," ",'Coéquipier 1'!D10:I10," = ",'Coéquipier 1'!F11:I25," ",'Coéquipier 1'!D27:I27,CHAR(10),'Coéquipier 2'!D9:I9," ",'Coéquipier 2'!D10:I10," = ",'Coéquipier 2'!F11:I25,CHAR(10),'Coéquipier 3'!D9:I9," ",'Coéquipier 3'!D10:I10," = ",'Coéquipier 3'!F11:I25,CHAR(10),'Coéquipier 4'!D9:I9," ",'Coéquipier 4'!D10:I10," = ",'Coéquipier 4'!F11:I25,CHAR(10),'Coéquipier 5'!D9:I9," ",'Coéquipier 5'!D10:I10," = ",'Coéquipier 5'!F11:I25)</f>
-        <v>Évaluateur = 73 Cette fois je suis beaucoup plus fier du résultat que j'ai produit. Je crois cependant que j'ai pris trop de temps a faire certaine tâche
-Louis Garceau = 73 La seul raison que j'ai pas mis 5 pour la ligne "a aidé l'équipe à prendre des décision" c'est parce qu'il n'a pas parlé tant que ça quand on parlais de ce a quoi on voulait qu'un module ressemble
+        <v>Évaluateur = 74 Toute la documentation que je devais produire à été complété à temps et j'ai même réussit à terminer des finitions dans l'applications dans les temps
+Louis Garceau = 74 La visualisation des résultats et ses tests ont été complété avec succès dans les temps. Il a même été retoucher certains de ses anciens développement pour simplifier la vie des utilisateurs
 Jean-Philippe Belval = 74
 Karl Mainville = 74
 Victor Turgeon = 74
@@ -1941,7 +1953,7 @@
       </c>
       <c r="C9" s="47">
         <f>SUM(C11:C466)</f>
-        <v>16.5</v>
+        <v>20</v>
       </c>
       <c r="D9" s="46" t="s">
         <v>64</v>
@@ -1966,31 +1978,31 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="48" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B11" s="49"/>
       <c r="C11" s="50">
         <v>0.75</v>
       </c>
       <c r="D11" s="49" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="48" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B12" s="52"/>
       <c r="C12" s="53">
         <v>4.25</v>
       </c>
       <c r="D12" s="52" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="48" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B13" s="52"/>
       <c r="C13" s="53">
@@ -2008,98 +2020,98 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="48" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B15" s="52"/>
       <c r="C15" s="53">
         <v>2</v>
       </c>
       <c r="D15" s="52" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="48" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B16" s="52"/>
       <c r="C16" s="53">
         <v>1</v>
       </c>
       <c r="D16" s="52" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="48" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B17" s="52"/>
       <c r="C17" s="53">
         <v>0.25</v>
       </c>
       <c r="D17" s="52" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="48" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B18" s="52"/>
       <c r="C18" s="53">
         <v>0.5</v>
       </c>
       <c r="D18" s="52" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="48" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B19" s="52"/>
       <c r="C19" s="53">
         <v>0.25</v>
       </c>
       <c r="D19" s="52" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="48" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B20" s="52"/>
       <c r="C20" s="53">
         <v>0.25</v>
       </c>
       <c r="D20" s="52" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="48" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B21" s="52"/>
       <c r="C21" s="53">
         <v>0.25</v>
       </c>
       <c r="D21" s="52" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="48" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B22" s="52"/>
       <c r="C22" s="53">
         <v>1</v>
       </c>
       <c r="D22" s="52" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -2110,50 +2122,50 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="48" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B24" s="52"/>
       <c r="C24" s="53">
         <v>0.25</v>
       </c>
       <c r="D24" s="52" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="48" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B25" s="52"/>
       <c r="C25" s="53">
         <v>0.75</v>
       </c>
       <c r="D25" s="52" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="48" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B26" s="52"/>
       <c r="C26" s="53">
         <v>4</v>
       </c>
       <c r="D26" s="52" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="48" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B27" s="52"/>
       <c r="C27" s="53">
         <v>0.5</v>
       </c>
       <c r="D27" s="52" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -2163,22 +2175,40 @@
       <c r="D28" s="52"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="51"/>
+      <c r="A29" s="48" t="s">
+        <v>95</v>
+      </c>
       <c r="B29" s="52"/>
-      <c r="C29" s="53"/>
-      <c r="D29" s="52"/>
+      <c r="C29" s="53">
+        <v>1</v>
+      </c>
+      <c r="D29" s="52" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="51"/>
+      <c r="A30" s="48" t="s">
+        <v>95</v>
+      </c>
       <c r="B30" s="52"/>
-      <c r="C30" s="53"/>
-      <c r="D30" s="52"/>
+      <c r="C30" s="53">
+        <v>2</v>
+      </c>
+      <c r="D30" s="52" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="51"/>
+      <c r="A31" s="48" t="s">
+        <v>95</v>
+      </c>
       <c r="B31" s="52"/>
-      <c r="C31" s="53"/>
-      <c r="D31" s="52"/>
+      <c r="C31" s="53">
+        <v>0.5</v>
+      </c>
+      <c r="D31" s="52" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="51"/>
@@ -4821,7 +4851,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14:I28"/>
+      <selection activeCell="D30" sqref="D30:I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5033,7 +5063,7 @@
       </c>
       <c r="F14" s="69">
         <f>IFERROR(SUM(E14:E28),"Autoévaluation à faire")</f>
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G14" s="70"/>
       <c r="H14" s="70"/>
@@ -5237,11 +5267,11 @@
         <v>15</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E25" s="13">
         <f>VLOOKUP(Évaluateur!D25,Menu!$B$4:$C$8,2,FALSE)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F25" s="72"/>
       <c r="G25" s="73"/>
@@ -5325,7 +5355,7 @@
         <v>1</v>
       </c>
       <c r="D30" s="64" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="E30" s="65"/>
       <c r="F30" s="65"/>
@@ -5442,7 +5472,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="D27" sqref="D27:I27"/>
     </sheetView>
   </sheetViews>
@@ -5605,7 +5635,7 @@
       </c>
       <c r="F11" s="80">
         <f>IFERROR(SUM(E11:E25),"à évaluer")</f>
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G11" s="81"/>
       <c r="H11" s="81"/>
@@ -5695,11 +5725,11 @@
         <v>36</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E16" s="13">
         <f>VLOOKUP('Coéquipier 1'!D16,Menu!$B$4:$C$8,2,FALSE)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F16" s="83"/>
       <c r="G16" s="84"/>
@@ -5897,7 +5927,7 @@
         <v>1</v>
       </c>
       <c r="D27" s="64" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="E27" s="65"/>
       <c r="F27" s="65"/>
@@ -6013,7 +6043,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="D27" sqref="D27:I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6467,7 +6497,7 @@
         <v>1</v>
       </c>
       <c r="D27" s="64" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="E27" s="65"/>
       <c r="F27" s="65"/>
@@ -7037,7 +7067,7 @@
         <v>1</v>
       </c>
       <c r="D27" s="64" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="E27" s="65"/>
       <c r="F27" s="65"/>
@@ -7153,7 +7183,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7607,7 +7637,7 @@
         <v>1</v>
       </c>
       <c r="D27" s="64" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="E27" s="65"/>
       <c r="F27" s="65"/>

</xml_diff>

<commit_message>
Documentation user et programmer
</commit_message>
<xml_diff>
--- a/FichesTemps/MaximeAubin4.xlsx
+++ b/FichesTemps/MaximeAubin4.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA30A006-D072-4498-A265-122E56408323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758A704C-B962-44C9-B9D7-CF7E4E66F429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="bsnEa0N1OcI6znPoPEcq3AHEi57LtmD/hoPfLk9LAHbO8ZgF/KxDU64xoRN551lSOgXhKiKNTKiOVsg9sOO7CQ==" workbookSaltValue="Arsw55Oy1Kl5wQ7vU+yWcQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="107">
   <si>
     <t>Fiche d'évaluation du travail d'équipe</t>
   </si>
@@ -461,6 +461,12 @@
   </si>
   <si>
     <t>Feuille de temps</t>
+  </si>
+  <si>
+    <t>Correction de la documentation</t>
+  </si>
+  <si>
+    <t>Documentation utilisateur pour la création de résultat</t>
   </si>
 </sst>
 </file>
@@ -1860,7 +1866,7 @@
   <dimension ref="A1:F466"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="E28" sqref="E28:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1953,7 +1959,7 @@
       </c>
       <c r="C9" s="47">
         <f>SUM(C11:C466)</f>
-        <v>20</v>
+        <v>22.75</v>
       </c>
       <c r="D9" s="46" t="s">
         <v>64</v>
@@ -2204,23 +2210,35 @@
       </c>
       <c r="B31" s="52"/>
       <c r="C31" s="53">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="D31" s="52" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="51"/>
+      <c r="A32" s="48" t="s">
+        <v>95</v>
+      </c>
       <c r="B32" s="52"/>
-      <c r="C32" s="53"/>
-      <c r="D32" s="52"/>
+      <c r="C32" s="53">
+        <v>1</v>
+      </c>
+      <c r="D32" s="52" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="51"/>
+      <c r="A33" s="48" t="s">
+        <v>95</v>
+      </c>
       <c r="B33" s="52"/>
-      <c r="C33" s="53"/>
-      <c r="D33" s="52"/>
+      <c r="C33" s="53">
+        <v>1.5</v>
+      </c>
+      <c r="D33" s="52" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="51"/>

</xml_diff>